<commit_message>
hey thats it de
</commit_message>
<xml_diff>
--- a/src/test/java/resorces/Practice.xlsx
+++ b/src/test/java/resorces/Practice.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="415">
   <si>
     <t xml:space="preserve"> United States</t>
   </si>
@@ -1710,9 +1710,7 @@
       <c r="A15" t="s">
         <v>26</v>
       </c>
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
+      <c r="B15"/>
     </row>
     <row r="16">
       <c r="A16" t="s">

</xml_diff>